<commit_message>
1nf, 2nf, 3nf and entity relationship diagram
</commit_message>
<xml_diff>
--- a/Database forms/Relationship diagram, normal forms.xlsx
+++ b/Database forms/Relationship diagram, normal forms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ohhja\Documents\Github\ParkingPriceSystem\Database forms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Novus\Project\ParkingPriceSystem\Database forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67CBEFF0-A83C-4AC2-B995-5CFAED7DD80B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91FC5432-25EF-463E-86C6-32549A03F217}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="20085" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="27">
   <si>
     <t>0NF</t>
   </si>
@@ -70,14 +70,67 @@
   </si>
   <si>
     <t>Station longitude</t>
+  </si>
+  <si>
+    <t>(Petrol Station Name</t>
+  </si>
+  <si>
+    <t>Last updated)</t>
+  </si>
+  <si>
+    <t>Last Updated</t>
+  </si>
+  <si>
+    <t>Fuel Type</t>
+  </si>
+  <si>
+    <t>User ID</t>
+  </si>
+  <si>
+    <t>StationID</t>
+  </si>
+  <si>
+    <t>*FuelPrice</t>
+  </si>
+  <si>
+    <t>USER</t>
+  </si>
+  <si>
+    <t>STATION</t>
+  </si>
+  <si>
+    <t>FUEL PRICE</t>
+  </si>
+  <si>
+    <t>Favourite Station</t>
+  </si>
+  <si>
+    <t>*StationID</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -105,8 +158,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -125,8 +181,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{171FD4B0-1C38-4E91-80AA-EDE030A75726}" name="Table2" displayName="Table2" ref="A1:E14" totalsRowShown="0">
-  <autoFilter ref="A1:E14" xr:uid="{171FD4B0-1C38-4E91-80AA-EDE030A75726}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{171FD4B0-1C38-4E91-80AA-EDE030A75726}" name="Table2" displayName="Table2" ref="A1:E21" totalsRowShown="0">
+  <autoFilter ref="A1:E21" xr:uid="{171FD4B0-1C38-4E91-80AA-EDE030A75726}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{883F59EB-2908-4946-8C26-9D628097FD23}" name="0NF"/>
     <tableColumn id="2" xr3:uid="{1598CDC8-F648-48D3-A721-57CCFD92D966}" name="1NF"/>
@@ -401,22 +457,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -433,54 +489,189 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>10</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>